<commit_message>
Adapt script - first successful trial
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vishesh\Documents\Python\YouTube\Whatsapp-Automation-Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/tbentze_worldbank_org/Documents/Documents/GitHub/Whatsapp-Automation-Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A514B16F-4C92-436C-8F90-3A8D6A3C27AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{A514B16F-4C92-436C-8F90-3A8D6A3C27AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECB58A8C-5ED0-43AE-8B85-62B73F4D5AF9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>SRNO</t>
   </si>
@@ -34,15 +47,31 @@
     <t>Message</t>
   </si>
   <si>
-    <t>Hi {{name}},
-This message that you are reading right now has been send automatically !!!
-To know how to do it, check out the channel 'All About Python'</t>
-  </si>
-  <si>
-    <t>Name of the receiver</t>
-  </si>
-  <si>
-    <t>Receiver whatsapp number</t>
+    <t>Thomas Bentze</t>
+  </si>
+  <si>
+    <t>+33621344207</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/World_Bank</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Pauline Castaing</t>
+  </si>
+  <si>
+    <t>+12027545429</t>
+  </si>
+  <si>
+    <t>Pauline Castaing number 2</t>
+  </si>
+  <si>
+    <t>+33664719529</t>
   </si>
 </sst>
 </file>
@@ -78,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -89,6 +118,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,10 +400,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="A1:D2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -377,7 +414,7 @@
     <col min="4" max="4" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -390,80 +427,185 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="60">
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="57" customHeight="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D2" s="5" t="str">
+        <f ca="1">_xlfn.CONCAT("Hi ",B2,", please click on the following link and enter the code", CHAR(10), "CODE: ",F2,CHAR(10),E2)</f>
+        <v>Hi Thomas Bentze, please click on the following link and enter the code
+CODE: 2812
+https://en.wikipedia.org/wiki/World_Bank</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(1000,9999)</f>
+        <v>2812</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="60">
+      <c r="A3" s="2">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <f ca="1">_xlfn.CONCAT("Hi ",B3,", please click on the following link and enter the code", CHAR(10), "CODE: ",F3,CHAR(10),E3)</f>
+        <v>Hi Pauline Castaing, please click on the following link and enter the code
+CODE: 4844
+https://en.wikipedia.org/wiki/World_Bank</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <f ca="1">RANDBETWEEN(1000,9999)</f>
+        <v>4844</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60">
+      <c r="A4" s="2">
+        <f t="shared" ref="A4:A21" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="str">
+        <f ca="1">_xlfn.CONCAT("Hi ",B4,", please click on the following link and enter the code", CHAR(10), "CODE: ",F4,CHAR(10),E4)</f>
+        <v>Hi Pauline Castaing number 2, please click on the following link and enter the code
+CODE: 5961
+https://en.wikipedia.org/wiki/World_Bank</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <f ca="1">RANDBETWEEN(1000,9999)</f>
+        <v>5961</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>